<commit_message>
added createOrder method 🤯
</commit_message>
<xml_diff>
--- a/diagrama-sql.xlsx
+++ b/diagrama-sql.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Enzo Sakamoto\Documents\repositorios_github\projeto-semestral-lp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB648AA8-1B61-4DE1-B969-DB8CC3542C02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B152E8D7-E531-4BC8-8AA9-D800C1752CCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C02D32C3-B9E7-4786-B3AB-3A24BCA62063}"/>
+    <workbookView xWindow="1605" yWindow="4905" windowWidth="24165" windowHeight="11295" xr2:uid="{C02D32C3-B9E7-4786-B3AB-3A24BCA62063}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -242,7 +242,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -280,6 +280,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -290,15 +293,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -617,8 +611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{483DBF33-8259-4D1B-ABAA-638041CADCB4}">
   <dimension ref="D4:L10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B4" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D4" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -645,13 +639,13 @@
       </c>
       <c r="J5" s="12"/>
       <c r="K5" s="12"/>
-      <c r="L5" s="17"/>
+      <c r="L5" s="13"/>
     </row>
     <row r="6" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="E6" s="14"/>
+      <c r="E6" s="15"/>
       <c r="F6" s="1" t="s">
         <v>4</v>
       </c>
@@ -670,10 +664,10 @@
       </c>
     </row>
     <row r="7" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="14"/>
+      <c r="E7" s="15"/>
       <c r="F7" s="1" t="s">
         <v>5</v>
       </c>
@@ -683,11 +677,11 @@
       <c r="H7" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="13" t="s">
+      <c r="I7" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="J7" s="18"/>
-      <c r="K7" s="19" t="s">
+      <c r="J7" s="15"/>
+      <c r="K7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="L7" s="3" t="s">
@@ -695,21 +689,21 @@
       </c>
     </row>
     <row r="8" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="14"/>
+      <c r="E8" s="15"/>
       <c r="F8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I8" s="13" t="s">
+      <c r="I8" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="18"/>
-      <c r="K8" s="19" t="s">
+      <c r="J8" s="15"/>
+      <c r="K8" s="1" t="s">
         <v>4</v>
       </c>
       <c r="L8" s="3" t="s">
@@ -717,21 +711,21 @@
       </c>
     </row>
     <row r="9" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D9" s="15" t="s">
+      <c r="D9" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="16"/>
+      <c r="E9" s="17"/>
       <c r="F9" s="4" t="s">
         <v>6</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I9" s="13" t="s">
+      <c r="I9" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="J9" s="18"/>
-      <c r="K9" s="19" t="s">
+      <c r="J9" s="15"/>
+      <c r="K9" s="1" t="s">
         <v>5</v>
       </c>
       <c r="L9" s="3" t="s">
@@ -739,10 +733,10 @@
       </c>
     </row>
     <row r="10" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I10" s="15" t="s">
+      <c r="I10" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="J10" s="16"/>
+      <c r="J10" s="17"/>
       <c r="K10" s="4" t="s">
         <v>17</v>
       </c>

</xml_diff>